<commit_message>
Updated Risk Assessment and README files
</commit_message>
<xml_diff>
--- a/Documentation/Risk Assessment.xlsx
+++ b/Documentation/Risk Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ridwa\Desktop\QA\QA Community\Projects\Software Core - Fundamental Project\IMS-22EnableMay2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E3ECCD-6B07-4B6E-99E5-BEACB2EB419C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690E418A-B7F7-4349-8210-E4215C08BDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t xml:space="preserve">No internet connectivity will ensure you can't access remote files or create backups on cloud hosted websites. </t>
   </si>
   <si>
-    <t>Employ the Feature-Branch Model (FBM) to organise your work and only merging the branches to your development branch when you feel like you reached a milestone/checkpoint/a working completion of a feature. If the work is to be done in a secure environment then using internet hotspot from a personal mobile phone is preferred.</t>
-  </si>
-  <si>
     <t>Reduces the severity and inconvenience caused by the loss of internet connectivity.</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t xml:space="preserve">To provide customers and clients with a sense of security and ensure that GDPR regulations are adhered to. </t>
   </si>
   <si>
-    <t>Having the means to a facility that offers reliable internet connection such as a café/library/academic environment could be employed to mitigate the risk. Changing Network providers or asking for a network engineer to resolve the issue.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Power cuts can lead to a loss of data, Can come without a warning and prevent one from accessing their pc's. It's a risk out of one's control and will need to be investigated by a third party, i.e. electricians. </t>
   </si>
   <si>
@@ -151,6 +145,12 @@
   </si>
   <si>
     <t>Since an IMS is being built, it is of utmost importance that data from the inventory system isn't breached. Could contain personal information such as one's names, contact numbers or even home address.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employ the Feature-Branch Model (FBM) to organise your work and only merging the branches to your development branch when you feel like you reached a milestone/checkpoint/a working completion of a feature. </t>
+  </si>
+  <si>
+    <t>Having the means to a facility that offers reliable internet connection such as a café/library/academic environment could be employed to mitigate the risk. Changing Network providers or asking for a network engineer to resolve the issue. If the work is to be done in a secure environment then using internet hotspot from a personal mobile phone is preferred.</t>
   </si>
 </sst>
 </file>
@@ -225,12 +225,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -241,9 +238,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
@@ -263,6 +257,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -567,280 +570,280 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15">
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="1" t="s">
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="2:15">
-      <c r="J3" s="8"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="2" t="s">
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O3" s="2" t="s">
+      <c r="N3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="30.5" customHeight="1">
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O4" s="4" t="s">
+      <c r="N4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="43.5">
-      <c r="K5" s="6"/>
-      <c r="L5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" s="5" t="s">
+      <c r="K5" s="13"/>
+      <c r="L5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="34" customHeight="1">
-      <c r="K6" s="6"/>
-      <c r="L6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="N6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="5" t="s">
+      <c r="K6" s="13"/>
+      <c r="L6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="2:15">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="101.5">
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="2:15" ht="110.5" customHeight="1">
+      <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" ht="118.5" customHeight="1">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" ht="173.5" customHeight="1">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="11" t="s">
+      <c r="E12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="101.5">
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" ht="117.5" customHeight="1">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="D14" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F14" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G10" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15" ht="101.5">
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="G14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" ht="96" customHeight="1">
+      <c r="B15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G11" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:15" ht="101.5">
-      <c r="B12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" s="12" t="s">
+      <c r="G15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" ht="127.5" customHeight="1">
+      <c r="B16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="131" customHeight="1">
+      <c r="B17" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H12" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="159.5">
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" ht="101.5">
-      <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" ht="87">
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="2:15" ht="101.5">
-      <c r="B16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" ht="116">
-      <c r="B17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="3" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>